<commit_message>
maven surefire plugin added
</commit_message>
<xml_diff>
--- a/src/main/java/TestData/TestData.xlsx
+++ b/src/main/java/TestData/TestData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="105" windowWidth="14295" windowHeight="4635"/>
+    <workbookView xWindow="0" yWindow="2520" windowWidth="14265" windowHeight="6330"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -12,6 +12,7 @@
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="124519"/>
+  <oleSize ref="A1"/>
 </workbook>
 </file>
 
@@ -356,7 +357,7 @@
   <dimension ref="A1:B1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>

</xml_diff>